<commit_message>
fix bom machinable file
</commit_message>
<xml_diff>
--- a/PK_MUV/Hardware/BOM.xlsx
+++ b/PK_MUV/Hardware/BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2020" yWindow="460" windowWidth="27680" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="1000" yWindow="460" windowWidth="27780" windowHeight="15940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="106">
   <si>
     <t>Description</t>
   </si>
@@ -78,12 +78,6 @@
   </si>
   <si>
     <t>https://nl.farnell.com/panasonic-electronic-components/erj8geyj103v/res-10k-5-0-25w-1206-thick-film/dp/2057856</t>
-  </si>
-  <si>
-    <t>SMD Chip Resistor, 470 kohm, RC Series, 200 V, Thick Film, 1206 [3216 Metric], 250 mW, 1%</t>
-  </si>
-  <si>
-    <t>https://nl.farnell.com/yageo/rc1206fr-07470kl/res-470k-1-0-25w-1206-thick-film/dp/9241108</t>
   </si>
   <si>
     <t>Transducer, Piezo, Leaded, min1 V, 8 mA, 90 dB, 5.5 kHz</t>
@@ -330,9 +324,6 @@
     <t>https://nl.farnell.com/amphenol-icc-fci/71600-104lf/connector-rcpt-4pos-2row-2-54mm/dp/2886085?ost=2886085&amp;scope=partnumberlookahead&amp;searchref=searchlookahead&amp;krypto=mwvLDoNLXKaxslTVzgSB6JoS3QtEV2hNPlC0xmGqv2u%2B1QqijtmsKCWDFKogv6Ke8CWa6Ov8bVnshOkiTSh2h6g%2BYQS3KdgWyJiEs3mEE4xsjLlG2J67u1a2AJj4XlZo6GHD45IPrVZEGbXw8YNBLVPLRCE21v9inJXBfmthTtRqwJjkrunBzbZK5VCEEu0Sv%2FLPCroqSoktEwFha2Dil0uoCK%2BjK8DIenW7sR7Kq%2Fa%2F51nAo4TTdOz4W98e5NoEm1cJYGG84MGD7t0I08BFCh3P8vZAjovm7nFtnd1c8TaJXBxrciwKCrP%2FrSRLLhXs20IgALQiSMYFgwD90CbqcmrbaRJVXp9jPkL%2Bfpep%2FKbciSXwT9ZL7Edtku4TiXUNlzs99f48VRiM7JdOf5uTta0CJVnHfuBoy2v22Hcf%2FaoIfI%2BBpogtDALLTtE6yJaPuQkg4uJ3r3evJhZZNKb3gk4e6vbtkZ29a%2BDYt59q8pvBvfZZXeXINQ4DwKPxnY2dRs76UKIE5yQ5Fj28rLckdM3IGuMqZiXHQP7MVGsxo48d23nHBlc8FL%2BbqqJMzVaUaRDHFM8CZzfWYn0wjEiZphTPVRJL7wpfmmOUaD1BUHM%3D&amp;ddkey=https%3Anl-NL%2FElement14_Netherlands%2Fw%2Fsearch</t>
   </si>
   <si>
-    <t>https://nl.farnell.com/pro-signal/abt-422-rc/piezo-transducer-leaded/dp/1300025?ost=1300025&amp;krypto=hB5T%2FXWeMKG9bPPgBgoJjF27sAWm98gJ5MUSwuXQA6l6LXf176bNDI0QMeIhpHzoPnOcqslIZX2T3gaAUSNCwx%2FmkAEnNtPDyp1C9QvYqcZszzIoeDqi7UGxI8EzkTDOFI3EgR1rBSb76OZ5P1F6xq9uWhNHzGqb6bD8mTYDICflxwXh4SrZkosWUXBfy0TbxOeBpwgEp0bKxia0MPJ0fTbV2JODY5XlxzAMkMO0QPPbAjRE4%2FosbCWutWxi%2BgHk06OS79J1GmPxJih%2BMQjsb8QHw3zOuLMnNXXEv5RrpSt5UcN4Z%2FtnfbsACLsHlM28xQ1R6kSB30j9ci8AU3NyPtmuyc1YCogX7SEGYWjVfl6QlkgtE2lnhMMGiEl%2FXB4jR%2BHYAgGDU33bWgGPKWIjBlzJgPkZ85L4%2B%2FV0LKN2zNWH2ZQd%2B7hsSDNFm3SMskLqAFdO9%2Fyhrcf9wFSYiDxYfg%3D%3D&amp;ddkey=https%3Anl-NL%2FElement14_Netherlands%2Fsearch</t>
-  </si>
-  <si>
     <t>Cost of 1 kit (euro)</t>
   </si>
   <si>
@@ -346,6 +337,15 @@
   </si>
   <si>
     <t>WS2812B RGB Led, Neopixel, package 5050</t>
+  </si>
+  <si>
+    <t>https://nl.farnell.com/pro-signal/abt-422-rc/piezo-transducer-leaded/dp/1300025?scope=partnumberlookahead&amp;ost=1300025&amp;searchref=searchlookahead&amp;exaMfpn=true&amp;ddkey=https%3Anl-NL%2FElement14_Netherlands%2Fw%2Fsearch</t>
+  </si>
+  <si>
+    <t>https://nl.farnell.com/yageo/rc1206fr-07470rl/res-470r-1-0-25w-1206-thick-film/dp/9240926?st=RC1206FR-07470RL</t>
+  </si>
+  <si>
+    <t>SMD Chip Resistor, 1206 [3216 Metric], 470 ohm, RC Series, 200 V, Thick Film, 250 mW</t>
   </si>
 </sst>
 </file>
@@ -719,10 +719,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K42"/>
+  <dimension ref="A1:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -741,30 +741,30 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B3">
-        <f>SUM(I7:I42)</f>
-        <v>111.66200000000002</v>
+        <f>SUM(I7:I41)</f>
+        <v>111.23800000000001</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B4">
-        <f>SUM(J7:J43)</f>
-        <v>43.809200000000004</v>
+        <f>SUM(J7:J42)</f>
+        <v>43.766800000000003</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="32" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>0</v>
@@ -785,10 +785,10 @@
         <v>6</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>2</v>
@@ -796,7 +796,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -805,10 +805,10 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G7">
         <v>19.95</v>
@@ -825,12 +825,12 @@
         <v>19.95</v>
       </c>
       <c r="K7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -839,7 +839,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F8" s="2">
         <v>10230</v>
@@ -859,21 +859,21 @@
         <v>4.95</v>
       </c>
       <c r="K8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D10">
         <v>1</v>
@@ -899,15 +899,15 @@
         <v>2.15</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D11">
         <v>1</v>
@@ -933,15 +933,15 @@
         <v>0.49099999999999999</v>
       </c>
       <c r="K11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D12">
         <v>1</v>
@@ -963,19 +963,19 @@
         <v>4.0200000000000005</v>
       </c>
       <c r="J12">
-        <f t="shared" ref="J12:J29" si="2">G12*D12</f>
+        <f t="shared" ref="J12:J28" si="2">G12*D12</f>
         <v>0.40200000000000002</v>
       </c>
       <c r="K12" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D13">
         <v>1</v>
@@ -1001,15 +1001,15 @@
         <v>1.2</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D14">
         <v>1</v>
@@ -1035,15 +1035,15 @@
         <v>0.71299999999999997</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D15">
         <v>1</v>
@@ -1069,15 +1069,15 @@
         <v>0.53</v>
       </c>
       <c r="K15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D16">
         <v>1</v>
@@ -1103,12 +1103,12 @@
         <v>0.39</v>
       </c>
       <c r="K16" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
         <v>10</v>
@@ -1142,7 +1142,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C18" t="s">
         <v>13</v>
@@ -1176,7 +1176,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
@@ -1205,12 +1205,12 @@
         <v>0.10649999999999998</v>
       </c>
       <c r="K19" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
         <v>15</v>
@@ -1244,10 +1244,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>17</v>
+        <v>105</v>
       </c>
       <c r="D21">
         <v>1</v>
@@ -1256,38 +1256,38 @@
         <v>3</v>
       </c>
       <c r="F21" s="2">
-        <v>9241108</v>
+        <v>9240926</v>
       </c>
       <c r="G21">
-        <v>8.0500000000000002E-2</v>
+        <v>7.3599999999999999E-2</v>
       </c>
       <c r="H21">
         <v>10</v>
       </c>
       <c r="I21">
-        <f t="shared" ref="I21:I28" si="6">H21*G21</f>
-        <v>0.80500000000000005</v>
+        <f t="shared" ref="I21:I27" si="6">H21*G21</f>
+        <v>0.73599999999999999</v>
       </c>
       <c r="J21">
         <f t="shared" si="2"/>
-        <v>8.0500000000000002E-2</v>
-      </c>
-      <c r="K21" t="s">
-        <v>18</v>
+        <v>7.3599999999999999E-2</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D23">
         <v>1</v>
@@ -1313,15 +1313,15 @@
         <v>0.32600000000000001</v>
       </c>
       <c r="K23" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D24">
         <v>1</v>
@@ -1347,360 +1347,360 @@
         <v>0.34599999999999997</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="19" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C25" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" s="5">
-        <v>1</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="2">
-        <v>1469963</v>
+        <v>102</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>101</v>
+      </c>
+      <c r="F25" s="8">
+        <v>10707</v>
       </c>
       <c r="G25" s="2">
-        <v>3.5499999999999997E-2</v>
-      </c>
-      <c r="H25" s="5">
+        <f>1.95/10</f>
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="H25">
         <v>10</v>
       </c>
       <c r="I25">
         <f t="shared" si="6"/>
-        <v>0.35499999999999998</v>
+        <v>1.9500000000000002</v>
       </c>
       <c r="J25">
         <f t="shared" si="2"/>
-        <v>3.5499999999999997E-2</v>
+        <v>0.19500000000000001</v>
       </c>
       <c r="K25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="2">
+        <v>2356177</v>
+      </c>
+      <c r="G27">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="H27">
+        <v>10</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="6"/>
+        <v>4.88</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="2"/>
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="K27" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" s="2">
+        <v>2429364</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="H28">
+        <v>5</v>
+      </c>
+      <c r="I28">
+        <f t="shared" ref="I28" si="7">H28*G28</f>
+        <v>1.73</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="2"/>
+        <v>0.69199999999999995</v>
+      </c>
+      <c r="K28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="19" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>56</v>
       </c>
-      <c r="C26" t="s">
-        <v>105</v>
-      </c>
-      <c r="D26">
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
-        <v>104</v>
-      </c>
-      <c r="F26" s="8">
+      <c r="C29" t="s">
+        <v>102</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>101</v>
+      </c>
+      <c r="F29" s="8">
         <v>10707</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G29" s="2">
         <f>1.95/10</f>
         <v>0.19500000000000001</v>
       </c>
-      <c r="H26">
+      <c r="H29">
         <v>10</v>
       </c>
-      <c r="I26">
-        <f t="shared" si="6"/>
+      <c r="I29">
+        <f t="shared" ref="I29" si="8">H29*G29</f>
         <v>1.9500000000000002</v>
       </c>
-      <c r="J26">
-        <f t="shared" si="2"/>
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="K26" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>54</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="J29">
+        <f t="shared" ref="J29" si="9">G29*D29</f>
+        <v>0.39</v>
+      </c>
+      <c r="K29" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>52</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31" s="2">
+        <v>2356217</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0.65400000000000003</v>
+      </c>
+      <c r="H31">
+        <v>10</v>
+      </c>
+      <c r="K31" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>3</v>
-      </c>
-      <c r="F28" s="2">
-        <v>2356177</v>
-      </c>
-      <c r="G28">
-        <v>0.48799999999999999</v>
-      </c>
-      <c r="H28">
-        <v>10</v>
-      </c>
-      <c r="I28">
-        <f t="shared" si="6"/>
-        <v>4.88</v>
-      </c>
-      <c r="J28">
-        <f t="shared" si="2"/>
-        <v>0.48799999999999999</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>57</v>
-      </c>
-      <c r="C29" t="s">
-        <v>62</v>
-      </c>
-      <c r="D29">
-        <v>2</v>
-      </c>
-      <c r="E29" t="s">
-        <v>3</v>
-      </c>
-      <c r="F29" s="2">
-        <v>2429364</v>
-      </c>
-      <c r="G29" s="2">
-        <v>0.34599999999999997</v>
-      </c>
-      <c r="H29">
-        <v>5</v>
-      </c>
-      <c r="I29">
-        <f t="shared" ref="I29" si="7">H29*G29</f>
-        <v>1.73</v>
-      </c>
-      <c r="J29">
-        <f t="shared" si="2"/>
-        <v>0.69199999999999995</v>
-      </c>
-      <c r="K29" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="19" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>58</v>
-      </c>
-      <c r="C30" t="s">
-        <v>105</v>
-      </c>
-      <c r="D30">
-        <v>2</v>
-      </c>
-      <c r="E30" t="s">
-        <v>104</v>
-      </c>
-      <c r="F30" s="8">
-        <v>10707</v>
-      </c>
-      <c r="G30" s="2">
-        <f>1.95/10</f>
-        <v>0.19500000000000001</v>
-      </c>
-      <c r="H30">
-        <v>10</v>
-      </c>
-      <c r="I30">
-        <f t="shared" ref="I30" si="8">H30*G30</f>
-        <v>1.9500000000000002</v>
-      </c>
-      <c r="J30">
-        <f t="shared" ref="J30" si="9">G30*D30</f>
-        <v>0.39</v>
-      </c>
-      <c r="K30" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>67</v>
+        <v>31</v>
+      </c>
+      <c r="C32" t="s">
+        <v>19</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E32" t="s">
         <v>3</v>
       </c>
       <c r="F32" s="2">
-        <v>2356217</v>
+        <v>2402405</v>
       </c>
       <c r="G32" s="2">
-        <v>0.65400000000000003</v>
+        <v>1.26</v>
       </c>
       <c r="H32">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="I32">
+        <f t="shared" ref="I32" si="10">H32*G32</f>
+        <v>6.3</v>
+      </c>
+      <c r="J32">
+        <f>G32*D32</f>
+        <v>2.52</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>66</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33">
-        <v>2</v>
-      </c>
-      <c r="E33" t="s">
-        <v>3</v>
-      </c>
-      <c r="F33" s="2">
-        <v>2402405</v>
-      </c>
-      <c r="G33" s="2">
-        <v>1.26</v>
-      </c>
-      <c r="H33">
-        <v>5</v>
-      </c>
-      <c r="I33">
-        <f t="shared" ref="I33" si="10">H33*G33</f>
-        <v>6.3</v>
-      </c>
-      <c r="J33">
-        <f>G33*D33</f>
-        <v>2.52</v>
-      </c>
-      <c r="K33" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="A33" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>65</v>
-      </c>
-      <c r="G34" s="2"/>
+      <c r="B34" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>87</v>
+      </c>
+      <c r="F34" s="2"/>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <f t="shared" ref="I34" si="11">H34*G34</f>
+        <v>0</v>
+      </c>
+      <c r="J34">
+        <f t="shared" ref="J34" si="12">G34*D34</f>
+        <v>0</v>
+      </c>
+      <c r="K34" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" t="s">
-        <v>93</v>
+        <v>71</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>89</v>
-      </c>
-      <c r="F35" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1123875</v>
+      </c>
+      <c r="G35">
+        <v>0.64500000000000002</v>
+      </c>
       <c r="H35">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I35">
-        <f t="shared" ref="I35" si="11">H35*G35</f>
-        <v>0</v>
+        <f t="shared" ref="I35:I38" si="13">H35*G35</f>
+        <v>3.2250000000000001</v>
       </c>
       <c r="J35">
-        <f t="shared" ref="J35" si="12">G35*D35</f>
-        <v>0</v>
+        <f t="shared" ref="J35:J38" si="14">G35*D35</f>
+        <v>0.64500000000000002</v>
       </c>
       <c r="K35" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>73</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>85</v>
+        <v>72</v>
+      </c>
+      <c r="C36" t="s">
+        <v>75</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>3</v>
-      </c>
-      <c r="F36" s="2">
-        <v>1123875</v>
-      </c>
-      <c r="G36">
-        <v>0.64500000000000002</v>
+        <v>76</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G36" s="2">
+        <v>2.25</v>
       </c>
       <c r="H36">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I36">
-        <f t="shared" ref="I36:I39" si="13">H36*G36</f>
-        <v>3.2250000000000001</v>
+        <f t="shared" si="13"/>
+        <v>2.25</v>
       </c>
       <c r="J36">
-        <f t="shared" ref="J36:J39" si="14">G36*D36</f>
-        <v>0.64500000000000002</v>
+        <f t="shared" si="14"/>
+        <v>2.25</v>
       </c>
       <c r="K36" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>78</v>
-      </c>
-      <c r="F37" s="7" t="s">
-        <v>81</v>
+        <v>3</v>
+      </c>
+      <c r="F37" s="2">
+        <v>9492615</v>
       </c>
       <c r="G37" s="2">
-        <v>2.25</v>
+        <v>0.46700000000000003</v>
       </c>
       <c r="H37">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I37">
         <f t="shared" si="13"/>
-        <v>2.25</v>
+        <v>4.67</v>
       </c>
       <c r="J37">
         <f t="shared" si="14"/>
-        <v>2.25</v>
+        <v>0.46700000000000003</v>
       </c>
       <c r="K37" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="D38">
         <v>1</v>
@@ -1709,142 +1709,110 @@
         <v>3</v>
       </c>
       <c r="F38" s="2">
-        <v>9492615</v>
-      </c>
-      <c r="G38" s="2">
-        <v>0.46700000000000003</v>
+        <v>1190779</v>
+      </c>
+      <c r="G38">
+        <v>1.21</v>
       </c>
       <c r="H38">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="I38">
         <f t="shared" si="13"/>
-        <v>4.67</v>
+        <v>6.05</v>
       </c>
       <c r="J38">
         <f t="shared" si="14"/>
-        <v>0.46700000000000003</v>
+        <v>1.21</v>
       </c>
       <c r="K38" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="A39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="D39">
-        <v>1</v>
-      </c>
-      <c r="E39" t="s">
-        <v>3</v>
-      </c>
-      <c r="F39" s="2">
-        <v>1190779</v>
-      </c>
-      <c r="G39">
-        <v>1.21</v>
-      </c>
-      <c r="H39">
-        <v>5</v>
-      </c>
-      <c r="I39">
-        <f t="shared" si="13"/>
-        <v>6.05</v>
-      </c>
-      <c r="J39">
-        <f t="shared" si="14"/>
-        <v>1.21</v>
-      </c>
-      <c r="K39" t="s">
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
+        <v>3</v>
+      </c>
+      <c r="F40" s="2">
+        <v>297318</v>
+      </c>
+      <c r="G40" s="2">
+        <v>2.34</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+      <c r="I40">
+        <f t="shared" ref="I40:I41" si="15">H40*G40</f>
+        <v>2.34</v>
+      </c>
+      <c r="J40">
+        <f t="shared" ref="J40:J41" si="16">G40*D40</f>
+        <v>2.34</v>
+      </c>
+      <c r="K40" t="s">
         <v>95</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>96</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E41" t="s">
         <v>3</v>
       </c>
       <c r="F41" s="2">
-        <v>297318</v>
+        <v>2886085</v>
       </c>
       <c r="G41" s="2">
-        <v>2.34</v>
+        <v>0.39100000000000001</v>
       </c>
       <c r="H41">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I41">
-        <f t="shared" ref="I41:I42" si="15">H41*G41</f>
-        <v>2.34</v>
+        <f t="shared" si="15"/>
+        <v>1.9550000000000001</v>
       </c>
       <c r="J41">
-        <f t="shared" ref="J41:J42" si="16">G41*D41</f>
-        <v>2.34</v>
+        <f t="shared" si="16"/>
+        <v>0.78200000000000003</v>
       </c>
       <c r="K41" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
-        <v>84</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D42">
-        <v>2</v>
-      </c>
-      <c r="E42" t="s">
-        <v>3</v>
-      </c>
-      <c r="F42" s="2">
-        <v>2886085</v>
-      </c>
-      <c r="G42" s="2">
-        <v>0.39100000000000001</v>
-      </c>
-      <c r="H42">
-        <v>5</v>
-      </c>
-      <c r="I42">
-        <f t="shared" si="15"/>
-        <v>1.9550000000000001</v>
-      </c>
-      <c r="J42">
-        <f t="shared" si="16"/>
-        <v>0.78200000000000003</v>
-      </c>
-      <c r="K42" t="s">
-        <v>99</v>
-      </c>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K33" r:id="rId1"/>
+    <hyperlink ref="K32" r:id="rId1"/>
     <hyperlink ref="K18" r:id="rId2"/>
     <hyperlink ref="K17" r:id="rId3"/>
-    <hyperlink ref="K28" r:id="rId4"/>
-    <hyperlink ref="K32" r:id="rId5"/>
+    <hyperlink ref="K27" r:id="rId4"/>
+    <hyperlink ref="K31" r:id="rId5"/>
     <hyperlink ref="K23" r:id="rId6"/>
     <hyperlink ref="K24" r:id="rId7"/>
+    <hyperlink ref="K10" r:id="rId8"/>
+    <hyperlink ref="K21" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>